<commit_message>
Atualização automática de SAO_LUIZ_GONZAGA.xlsx
</commit_message>
<xml_diff>
--- a/SAO_LUIZ_GONZAGA.xlsx
+++ b/SAO_LUIZ_GONZAGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F6B9BD-2C0C-4EE5-BECD-1110FD061FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C93AF63-F93A-4DB3-B25B-4379489DAEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1188,7 +1188,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{2B6E4AD1-3DA6-4D80-A93F-71779CB29D12}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{64785856-DA3F-413B-8B59-FFAFA4ED9E9F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1218,10 +1218,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA2D0AF9-E362-417D-B147-0FEE0D7AEEDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADCC05F8-C27B-41E9-867F-79A6013FE0CE}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1259,7 +1259,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B8EB027-E6A1-4BFA-B669-195606696A53}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B71CD49C-4401-4281-B744-FE1499964B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1322,7 +1322,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BDC2A80-2BD0-4834-B55F-EDE04938780F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E52988CF-06D4-4A04-98DF-7FBFB9F7E686}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1341,7 +1341,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{877C0888-93F0-6662-E651-92E7FC4684FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FDB532A-D6AF-DE5C-3BBD-38191C80B8EB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1390,7 +1390,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{502E1721-F486-41D3-6B21-71C581A09136}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1303D2EA-22E2-939F-8F32-0E2CF4E461A5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1409,7 +1409,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3083A4C7-9982-7A05-E4A8-862C196C0C2C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2CD4490-F7E8-A58E-7FA4-BC7A9984FA43}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1440,7 +1440,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B348B272-0842-6153-9D66-BEA9C6BA28E7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C06E5388-54FA-0BD8-6975-81014B95C8D9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{874DC88D-3786-DF90-1AC9-87C23C077225}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9766D049-511C-DABA-2F4C-6728AF2F0661}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1514,7 +1514,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{904ADF5D-4713-411C-A9AE-A5D4FA181F5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8B6605C-67F1-44C4-BEAC-CFA876914BD1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1552,7 +1552,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8290F7C4-9926-42F9-9E34-9652645E5DAB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82BFFED8-123D-4562-9959-1F895B221F5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1595,7 +1595,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAC1DD78-1DB0-41D4-A3D2-6772F7D72B74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34B1895A-B8F3-4B1C-9E0C-3F9C8D5B999B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1908,7 +1908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219CFBB5-4DA6-4B9F-8DD6-AA59C0FC35E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389AB20F-0507-4D14-8FCC-C97BE40BD209}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>